<commit_message>
Revisione overview + incremento Sprint 1
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Workplan.xlsx
+++ b/DOCUMENTS/Workplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\LORI\UNIVERSITA'\Magistrale\2°Anno\II Ciclo\Ingegneria dei Sistemi Software\Waiter_Robot\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E194E1B-B391-4CC3-95ED-9D869859B6D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15B9DFD-FDE8-435A-8341-E1684B45A2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="59">
   <si>
     <t>Sprint Goal (obiettivo)</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Analisi del Problema (+ Creazione del modello eseguibile)</t>
-  </si>
-  <si>
     <t>Realizzazione del planner</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>Gestione "non ottimizzata" di più clienti</t>
   </si>
   <si>
-    <t>Implementazione della Web Application</t>
-  </si>
-  <si>
     <t>Ottimizzazione del waiter</t>
   </si>
   <si>
@@ -211,6 +205,15 @@
   </si>
   <si>
     <t>Robot in grado di muoversi all'interno della Tea Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementare </t>
+  </si>
+  <si>
+    <t>Analisi del Problema (+ creazione del modello eseguibile)</t>
+  </si>
+  <si>
+    <t>Implementazione della Web Application (e della current Situation)</t>
   </si>
 </sst>
 </file>
@@ -584,10 +587,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,66 +612,60 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -668,64 +677,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1312,7 +1315,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,7 +1348,7 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1389,6 +1392,9 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1454,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6357E3-4FBB-418C-9BB3-004C68F042FF}">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1472,14 +1478,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
+      <c r="A1" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1504,27 +1510,27 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="88" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="54"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="88" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
-      <c r="B4" s="99"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="90"/>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
@@ -1533,11 +1539,11 @@
       <c r="F4" s="11">
         <v>44002</v>
       </c>
-      <c r="G4" s="66"/>
+      <c r="G4" s="88"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="100"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="91"/>
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1548,13 +1554,13 @@
       <c r="F5" s="11">
         <v>44003</v>
       </c>
-      <c r="G5" s="66"/>
+      <c r="G5" s="88"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
-      <c r="B6" s="100"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="91"/>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="4" t="s">
@@ -1563,13 +1569,13 @@
       <c r="F6" s="11">
         <v>44004</v>
       </c>
-      <c r="G6" s="66"/>
+      <c r="G6" s="88"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="66"/>
-      <c r="B7" s="101"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="s">
@@ -1578,154 +1584,154 @@
       <c r="F7" s="65">
         <v>44005</v>
       </c>
-      <c r="G7" s="66"/>
+      <c r="G7" s="88"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="67">
+      <c r="A8" s="81">
         <v>1</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="67"/>
+      <c r="G8" s="81"/>
     </row>
     <row r="9" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="96" t="s">
-        <v>52</v>
+      <c r="A9" s="81"/>
+      <c r="B9" s="76" t="s">
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="91"/>
+      <c r="D9" s="93"/>
       <c r="E9" s="4"/>
       <c r="F9" s="11">
         <v>44006</v>
       </c>
-      <c r="G9" s="67"/>
+      <c r="G9" s="81"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="97"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="92"/>
+        <v>57</v>
+      </c>
+      <c r="D10" s="94"/>
       <c r="E10" s="4"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="67"/>
+      <c r="G10" s="81"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="97"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="92"/>
+      <c r="D11" s="94"/>
       <c r="E11" s="4"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="67"/>
+      <c r="G11" s="81"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="97"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="92"/>
+        <v>38</v>
+      </c>
+      <c r="D12" s="94"/>
       <c r="E12" s="4"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="67"/>
+      <c r="G12" s="81"/>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
-      <c r="B13" s="97"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="92"/>
+        <v>40</v>
+      </c>
+      <c r="D13" s="94"/>
       <c r="E13" s="4"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="67"/>
+      <c r="G13" s="81"/>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
-      <c r="B14" s="97"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="79"/>
       <c r="C14" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="92"/>
+        <v>39</v>
+      </c>
+      <c r="D14" s="94"/>
       <c r="E14" s="4"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="67"/>
+      <c r="G14" s="81"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="97"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="92"/>
+        <v>37</v>
+      </c>
+      <c r="D15" s="94"/>
       <c r="E15" s="4"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="67"/>
+      <c r="G15" s="81"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="98"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="94"/>
       <c r="E16" s="4"/>
       <c r="F16" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="67"/>
+        <v>53</v>
+      </c>
+      <c r="G16" s="81"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="67"/>
+      <c r="A17" s="81"/>
       <c r="B17" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="92"/>
+      <c r="D17" s="94"/>
       <c r="E17" s="4"/>
-      <c r="G17" s="67"/>
+      <c r="G17" s="81"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
+      <c r="A18" s="81"/>
       <c r="B18" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="92"/>
+      <c r="D18" s="94"/>
       <c r="E18" s="4"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="67"/>
+      <c r="G18" s="81"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
+      <c r="A19" s="81"/>
       <c r="B19" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="93"/>
+      <c r="D19" s="95"/>
       <c r="E19" s="4"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="67"/>
+      <c r="G19" s="81"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="84">
+      <c r="A20" s="80">
         <v>2</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>34</v>
@@ -1733,309 +1739,309 @@
       <c r="D20" s="55"/>
       <c r="E20" s="19"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="84"/>
+      <c r="G20" s="80"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
-      <c r="B21" s="96" t="s">
-        <v>52</v>
+      <c r="A21" s="80"/>
+      <c r="B21" s="76" t="s">
+        <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="91"/>
+      <c r="D21" s="93"/>
       <c r="E21" s="4"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="84"/>
+      <c r="G21" s="80"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
-      <c r="B22" s="97"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="79"/>
       <c r="C22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="92"/>
+        <v>43</v>
+      </c>
+      <c r="D22" s="94"/>
       <c r="E22" s="4"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="84"/>
+      <c r="G22" s="80"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
-      <c r="B23" s="97"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="79"/>
       <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="92"/>
+      <c r="D23" s="94"/>
       <c r="E23" s="4"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="84"/>
+      <c r="G23" s="80"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
-      <c r="B24" s="97"/>
+      <c r="A24" s="80"/>
+      <c r="B24" s="79"/>
       <c r="C24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="92"/>
+        <v>38</v>
+      </c>
+      <c r="D24" s="94"/>
       <c r="E24" s="4"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="84"/>
+      <c r="G24" s="80"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
-      <c r="B25" s="97"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="79"/>
       <c r="C25" s="64"/>
-      <c r="D25" s="92"/>
+      <c r="D25" s="94"/>
       <c r="E25" s="4"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="84"/>
+      <c r="G25" s="80"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
-      <c r="B26" s="97"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="79"/>
       <c r="C26" s="63"/>
-      <c r="D26" s="92"/>
+      <c r="D26" s="94"/>
       <c r="E26" s="4"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="84"/>
+      <c r="G26" s="80"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="97"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="79"/>
       <c r="C27" s="62"/>
-      <c r="D27" s="92"/>
+      <c r="D27" s="94"/>
       <c r="E27" s="4"/>
       <c r="F27" s="16"/>
-      <c r="G27" s="84"/>
+      <c r="G27" s="80"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
-      <c r="B28" s="98"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="92"/>
+      <c r="D28" s="94"/>
       <c r="E28" s="4"/>
       <c r="F28" s="16">
         <v>44014</v>
       </c>
-      <c r="G28" s="84"/>
+      <c r="G28" s="80"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="80"/>
       <c r="B29" s="50" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="92"/>
+      <c r="D29" s="94"/>
       <c r="E29" s="4"/>
       <c r="F29" s="16"/>
-      <c r="G29" s="84"/>
+      <c r="G29" s="80"/>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="84"/>
+      <c r="A30" s="80"/>
       <c r="B30" s="60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="92"/>
+      <c r="D30" s="94"/>
       <c r="E30" s="4"/>
       <c r="F30" s="16"/>
-      <c r="G30" s="84"/>
+      <c r="G30" s="80"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="84"/>
+      <c r="A31" s="80"/>
       <c r="B31" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="93"/>
+      <c r="D31" s="95"/>
       <c r="E31" s="4"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="84"/>
+      <c r="G31" s="80"/>
     </row>
     <row r="32" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="95">
+      <c r="A32" s="89">
         <v>3</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="23"/>
       <c r="F32" s="24"/>
-      <c r="G32" s="68"/>
+      <c r="G32" s="72"/>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="95"/>
-      <c r="B33" s="96" t="s">
-        <v>52</v>
+      <c r="A33" s="89"/>
+      <c r="B33" s="76" t="s">
+        <v>50</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="91"/>
+      <c r="D33" s="93"/>
       <c r="E33" s="4"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="69"/>
+      <c r="G33" s="73"/>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A34" s="95"/>
-      <c r="B34" s="97"/>
+      <c r="A34" s="89"/>
+      <c r="B34" s="79"/>
       <c r="C34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="92"/>
+        <v>43</v>
+      </c>
+      <c r="D34" s="94"/>
       <c r="E34" s="4"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="69"/>
+      <c r="G34" s="73"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="95"/>
-      <c r="B35" s="97"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="79"/>
       <c r="C35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="92"/>
+      <c r="D35" s="94"/>
       <c r="E35" s="4"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="69"/>
+      <c r="G35" s="73"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="95"/>
-      <c r="B36" s="97"/>
+      <c r="A36" s="89"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="92"/>
+        <v>38</v>
+      </c>
+      <c r="D36" s="94"/>
       <c r="E36" s="4"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="69"/>
+      <c r="G36" s="73"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="95"/>
-      <c r="B37" s="97"/>
+      <c r="A37" s="89"/>
+      <c r="B37" s="79"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="92"/>
+      <c r="D37" s="94"/>
       <c r="E37" s="4"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="69"/>
+      <c r="G37" s="73"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="95"/>
-      <c r="B38" s="98"/>
+      <c r="A38" s="89"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="92"/>
+      <c r="D38" s="94"/>
       <c r="E38" s="4"/>
       <c r="F38" s="16">
         <v>44018</v>
       </c>
-      <c r="G38" s="69"/>
+      <c r="G38" s="73"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="95"/>
+      <c r="A39" s="89"/>
       <c r="B39" s="50" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="63"/>
-      <c r="D39" s="92"/>
+      <c r="D39" s="94"/>
       <c r="E39" s="4"/>
       <c r="F39" s="16"/>
-      <c r="G39" s="69"/>
+      <c r="G39" s="73"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="95"/>
+      <c r="A40" s="89"/>
       <c r="B40" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40" s="64"/>
-      <c r="D40" s="92"/>
+      <c r="D40" s="94"/>
       <c r="E40" s="4"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="69"/>
+      <c r="G40" s="73"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="95"/>
+      <c r="A41" s="89"/>
       <c r="B41" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="93"/>
+      <c r="D41" s="95"/>
       <c r="E41" s="4"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="70"/>
+      <c r="G41" s="74"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="102">
+      <c r="A42" s="82">
         <v>4</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="27"/>
       <c r="F42" s="28"/>
-      <c r="G42" s="71"/>
+      <c r="G42" s="108"/>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="102"/>
-      <c r="B43" s="77" t="s">
-        <v>52</v>
+      <c r="A43" s="82"/>
+      <c r="B43" s="75" t="s">
+        <v>50</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="4"/>
       <c r="F43" s="16"/>
-      <c r="G43" s="72"/>
+      <c r="G43" s="109"/>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="102"/>
-      <c r="B44" s="77"/>
+      <c r="A44" s="82"/>
+      <c r="B44" s="75"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="4"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="72"/>
+      <c r="G44" s="109"/>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="102"/>
-      <c r="B45" s="77"/>
+      <c r="A45" s="82"/>
+      <c r="B45" s="75"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="4"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="72"/>
+      <c r="G45" s="109"/>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="102"/>
-      <c r="B46" s="77"/>
+      <c r="A46" s="82"/>
+      <c r="B46" s="75"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="4"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="72"/>
+      <c r="G46" s="109"/>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="102"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="82"/>
+      <c r="B47" s="75"/>
       <c r="C47" s="61"/>
       <c r="D47" s="61"/>
       <c r="E47" s="4"/>
       <c r="F47" s="16">
         <v>44022</v>
       </c>
-      <c r="G47" s="72"/>
+      <c r="G47" s="109"/>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="102"/>
+      <c r="A48" s="82"/>
       <c r="B48" s="50" t="s">
         <v>7</v>
       </c>
@@ -2043,21 +2049,21 @@
       <c r="D48" s="2"/>
       <c r="E48" s="4"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="72"/>
+      <c r="G48" s="109"/>
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="102"/>
+      <c r="A49" s="82"/>
       <c r="B49" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="4"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="72"/>
+      <c r="G49" s="109"/>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" s="102"/>
+      <c r="A50" s="82"/>
       <c r="B50" s="50" t="s">
         <v>8</v>
       </c>
@@ -2065,27 +2071,27 @@
       <c r="D50" s="2"/>
       <c r="E50" s="4"/>
       <c r="F50" s="16"/>
-      <c r="G50" s="73"/>
+      <c r="G50" s="110"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="103">
+      <c r="A51" s="83">
         <v>5</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="31"/>
       <c r="F51" s="32"/>
-      <c r="G51" s="74"/>
+      <c r="G51" s="111"/>
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="103"/>
-      <c r="B52" s="77" t="s">
-        <v>52</v>
+      <c r="A52" s="83"/>
+      <c r="B52" s="75" t="s">
+        <v>50</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>35</v>
@@ -2093,44 +2099,44 @@
       <c r="D52" s="2"/>
       <c r="E52" s="4"/>
       <c r="F52" s="16"/>
-      <c r="G52" s="75"/>
+      <c r="G52" s="112"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="103"/>
-      <c r="B53" s="77"/>
+      <c r="A53" s="83"/>
+      <c r="B53" s="75"/>
       <c r="C53" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="4"/>
       <c r="F53" s="16"/>
-      <c r="G53" s="75"/>
+      <c r="G53" s="112"/>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="103"/>
-      <c r="B54" s="77"/>
+      <c r="A54" s="83"/>
+      <c r="B54" s="75"/>
       <c r="C54" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="4"/>
       <c r="F54" s="16"/>
-      <c r="G54" s="75"/>
+      <c r="G54" s="112"/>
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="103"/>
-      <c r="B55" s="77"/>
+      <c r="A55" s="83"/>
+      <c r="B55" s="75"/>
       <c r="C55" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="4"/>
       <c r="F55" s="16"/>
-      <c r="G55" s="75"/>
+      <c r="G55" s="112"/>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="103"/>
-      <c r="B56" s="77"/>
+      <c r="A56" s="83"/>
+      <c r="B56" s="75"/>
       <c r="C56" s="2" t="s">
         <v>36</v>
       </c>
@@ -2139,10 +2145,10 @@
       <c r="F56" s="16">
         <v>44026</v>
       </c>
-      <c r="G56" s="75"/>
+      <c r="G56" s="112"/>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="103"/>
+      <c r="A57" s="83"/>
       <c r="B57" s="50" t="s">
         <v>7</v>
       </c>
@@ -2150,21 +2156,21 @@
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="75"/>
+      <c r="G57" s="112"/>
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A58" s="103"/>
+      <c r="A58" s="83"/>
       <c r="B58" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="2"/>
       <c r="E58" s="4"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="75"/>
+      <c r="G58" s="112"/>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="103"/>
+      <c r="A59" s="83"/>
       <c r="B59" s="50" t="s">
         <v>8</v>
       </c>
@@ -2172,54 +2178,54 @@
       <c r="D59" s="2"/>
       <c r="E59" s="4"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="76"/>
+      <c r="G59" s="113"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="104">
+      <c r="A60" s="84">
         <v>6</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C60" s="49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D60" s="49"/>
       <c r="E60" s="33"/>
       <c r="F60" s="34"/>
-      <c r="G60" s="85"/>
+      <c r="G60" s="102"/>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" s="104"/>
-      <c r="B61" s="77" t="s">
-        <v>52</v>
+      <c r="A61" s="84"/>
+      <c r="B61" s="75" t="s">
+        <v>50</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="4"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="86"/>
+      <c r="G61" s="103"/>
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A62" s="104"/>
-      <c r="B62" s="77"/>
+      <c r="A62" s="84"/>
+      <c r="B62" s="75"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="4"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="86"/>
+      <c r="G62" s="103"/>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="104"/>
-      <c r="B63" s="77"/>
+      <c r="A63" s="84"/>
+      <c r="B63" s="75"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="4"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="86"/>
+      <c r="G63" s="103"/>
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" s="104"/>
+      <c r="A64" s="84"/>
       <c r="B64" s="50" t="s">
         <v>7</v>
       </c>
@@ -2227,21 +2233,21 @@
       <c r="D64" s="2"/>
       <c r="E64" s="4"/>
       <c r="F64" s="16"/>
-      <c r="G64" s="86"/>
+      <c r="G64" s="103"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="104"/>
+      <c r="A65" s="84"/>
       <c r="B65" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="4"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="86"/>
+      <c r="G65" s="103"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="104"/>
+      <c r="A66" s="84"/>
       <c r="B66" s="50" t="s">
         <v>8</v>
       </c>
@@ -2249,52 +2255,52 @@
       <c r="D66" s="2"/>
       <c r="E66" s="4"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="87"/>
+      <c r="G66" s="104"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="105">
+      <c r="A67" s="85">
         <v>6</v>
       </c>
       <c r="B67" s="35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C67" s="36"/>
       <c r="D67" s="36"/>
       <c r="E67" s="37"/>
       <c r="F67" s="37"/>
-      <c r="G67" s="88"/>
+      <c r="G67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A68" s="105"/>
-      <c r="B68" s="77" t="s">
-        <v>52</v>
+      <c r="A68" s="85"/>
+      <c r="B68" s="75" t="s">
+        <v>50</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="4"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="89"/>
+      <c r="G68" s="106"/>
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="105"/>
-      <c r="B69" s="77"/>
+      <c r="A69" s="85"/>
+      <c r="B69" s="75"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="4"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="89"/>
+      <c r="G69" s="106"/>
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A70" s="105"/>
-      <c r="B70" s="77"/>
+      <c r="A70" s="85"/>
+      <c r="B70" s="75"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="4"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="89"/>
+      <c r="G70" s="106"/>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A71" s="105"/>
+      <c r="A71" s="85"/>
       <c r="B71" s="50" t="s">
         <v>7</v>
       </c>
@@ -2302,21 +2308,21 @@
       <c r="D71" s="2"/>
       <c r="E71" s="4"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="89"/>
+      <c r="G71" s="106"/>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="105"/>
+      <c r="A72" s="85"/>
       <c r="B72" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="4"/>
       <c r="F72" s="16"/>
-      <c r="G72" s="89"/>
+      <c r="G72" s="106"/>
     </row>
     <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A73" s="105"/>
+      <c r="A73" s="85"/>
       <c r="B73" s="50" t="s">
         <v>8</v>
       </c>
@@ -2324,52 +2330,52 @@
       <c r="D73" s="2"/>
       <c r="E73" s="4"/>
       <c r="F73" s="16"/>
-      <c r="G73" s="90"/>
+      <c r="G73" s="107"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="106">
+      <c r="A74" s="86">
         <v>7</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C74" s="39"/>
       <c r="D74" s="39"/>
       <c r="E74" s="40"/>
       <c r="F74" s="41"/>
-      <c r="G74" s="81"/>
+      <c r="G74" s="99"/>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A75" s="106"/>
-      <c r="B75" s="77" t="s">
-        <v>52</v>
+      <c r="A75" s="86"/>
+      <c r="B75" s="75" t="s">
+        <v>50</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="4"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="82"/>
+      <c r="G75" s="100"/>
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A76" s="106"/>
-      <c r="B76" s="77"/>
+      <c r="A76" s="86"/>
+      <c r="B76" s="75"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="4"/>
       <c r="F76" s="16"/>
-      <c r="G76" s="82"/>
+      <c r="G76" s="100"/>
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A77" s="106"/>
-      <c r="B77" s="77"/>
+      <c r="A77" s="86"/>
+      <c r="B77" s="75"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="4"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="82"/>
+      <c r="G77" s="100"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A78" s="106"/>
+      <c r="A78" s="86"/>
       <c r="B78" s="50" t="s">
         <v>7</v>
       </c>
@@ -2377,21 +2383,21 @@
       <c r="D78" s="2"/>
       <c r="E78" s="4"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="82"/>
+      <c r="G78" s="100"/>
     </row>
     <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A79" s="106"/>
+      <c r="A79" s="86"/>
       <c r="B79" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="4"/>
       <c r="F79" s="16"/>
-      <c r="G79" s="82"/>
+      <c r="G79" s="100"/>
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A80" s="106"/>
+      <c r="A80" s="86"/>
       <c r="B80" s="50" t="s">
         <v>8</v>
       </c>
@@ -2399,10 +2405,10 @@
       <c r="D80" s="2"/>
       <c r="E80" s="4"/>
       <c r="F80" s="16"/>
-      <c r="G80" s="83"/>
+      <c r="G80" s="101"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="107">
+      <c r="A81" s="78">
         <v>8</v>
       </c>
       <c r="B81" s="42" t="s">
@@ -2412,30 +2418,30 @@
       <c r="D81" s="43"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
-      <c r="G81" s="78"/>
+      <c r="G81" s="96"/>
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A82" s="107"/>
-      <c r="B82" s="77" t="s">
-        <v>52</v>
+      <c r="A82" s="78"/>
+      <c r="B82" s="75" t="s">
+        <v>50</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="4"/>
       <c r="F82" s="16"/>
-      <c r="G82" s="79"/>
+      <c r="G82" s="97"/>
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A83" s="107"/>
-      <c r="B83" s="77"/>
+      <c r="A83" s="78"/>
+      <c r="B83" s="75"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="4"/>
       <c r="F83" s="16"/>
-      <c r="G83" s="79"/>
+      <c r="G83" s="97"/>
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A84" s="107"/>
+      <c r="A84" s="78"/>
       <c r="B84" s="50" t="s">
         <v>7</v>
       </c>
@@ -2443,21 +2449,21 @@
       <c r="D84" s="2"/>
       <c r="E84" s="4"/>
       <c r="F84" s="16"/>
-      <c r="G84" s="79"/>
+      <c r="G84" s="97"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A85" s="107"/>
+      <c r="A85" s="78"/>
       <c r="B85" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="4"/>
       <c r="F85" s="16"/>
-      <c r="G85" s="79"/>
+      <c r="G85" s="97"/>
     </row>
     <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A86" s="107"/>
+      <c r="A86" s="78"/>
       <c r="B86" s="50" t="s">
         <v>8</v>
       </c>
@@ -2465,10 +2471,10 @@
       <c r="D86" s="2"/>
       <c r="E86" s="4"/>
       <c r="F86" s="16"/>
-      <c r="G86" s="80"/>
+      <c r="G86" s="98"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="67">
+      <c r="A87" s="81">
         <v>9</v>
       </c>
       <c r="B87" s="12" t="s">
@@ -2478,39 +2484,39 @@
       <c r="D87" s="13"/>
       <c r="E87" s="14"/>
       <c r="F87" s="15"/>
-      <c r="G87" s="108"/>
+      <c r="G87" s="66"/>
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A88" s="67"/>
-      <c r="B88" s="77" t="s">
-        <v>52</v>
+      <c r="A88" s="81"/>
+      <c r="B88" s="75" t="s">
+        <v>50</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="4"/>
       <c r="F88" s="16"/>
-      <c r="G88" s="109"/>
+      <c r="G88" s="67"/>
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A89" s="67"/>
-      <c r="B89" s="77"/>
+      <c r="A89" s="81"/>
+      <c r="B89" s="75"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="4"/>
       <c r="F89" s="16"/>
-      <c r="G89" s="109"/>
+      <c r="G89" s="67"/>
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A90" s="67"/>
-      <c r="B90" s="77"/>
+      <c r="A90" s="81"/>
+      <c r="B90" s="75"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="4"/>
       <c r="F90" s="16"/>
-      <c r="G90" s="109"/>
+      <c r="G90" s="67"/>
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="67"/>
+      <c r="A91" s="81"/>
       <c r="B91" s="50" t="s">
         <v>7</v>
       </c>
@@ -2518,21 +2524,21 @@
       <c r="D91" s="2"/>
       <c r="E91" s="4"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="109"/>
+      <c r="G91" s="67"/>
     </row>
     <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A92" s="67"/>
+      <c r="A92" s="81"/>
       <c r="B92" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="4"/>
       <c r="F92" s="16"/>
-      <c r="G92" s="109"/>
+      <c r="G92" s="67"/>
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A93" s="67"/>
+      <c r="A93" s="81"/>
       <c r="B93" s="50" t="s">
         <v>8</v>
       </c>
@@ -2540,10 +2546,10 @@
       <c r="D93" s="2"/>
       <c r="E93" s="4"/>
       <c r="F93" s="16"/>
-      <c r="G93" s="110"/>
+      <c r="G93" s="68"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="84">
+      <c r="A94" s="80">
         <v>10</v>
       </c>
       <c r="B94" s="46" t="s">
@@ -2553,30 +2559,30 @@
       <c r="D94" s="47"/>
       <c r="E94" s="19"/>
       <c r="F94" s="20"/>
-      <c r="G94" s="111"/>
+      <c r="G94" s="69"/>
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A95" s="84"/>
-      <c r="B95" s="96" t="s">
-        <v>52</v>
+      <c r="A95" s="80"/>
+      <c r="B95" s="76" t="s">
+        <v>50</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="4"/>
       <c r="F95" s="16"/>
-      <c r="G95" s="112"/>
+      <c r="G95" s="70"/>
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A96" s="84"/>
-      <c r="B96" s="98"/>
+      <c r="A96" s="80"/>
+      <c r="B96" s="77"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
       <c r="F96" s="16"/>
-      <c r="G96" s="112"/>
+      <c r="G96" s="70"/>
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A97" s="84"/>
+      <c r="A97" s="80"/>
       <c r="B97" s="50" t="s">
         <v>7</v>
       </c>
@@ -2584,21 +2590,21 @@
       <c r="D97" s="2"/>
       <c r="E97" s="4"/>
       <c r="F97" s="16"/>
-      <c r="G97" s="112"/>
+      <c r="G97" s="70"/>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A98" s="84"/>
+      <c r="A98" s="80"/>
       <c r="B98" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="4"/>
       <c r="F98" s="16"/>
-      <c r="G98" s="112"/>
+      <c r="G98" s="70"/>
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A99" s="84"/>
+      <c r="A99" s="80"/>
       <c r="B99" s="50" t="s">
         <v>8</v>
       </c>
@@ -2606,10 +2612,10 @@
       <c r="D99" s="2"/>
       <c r="E99" s="4"/>
       <c r="F99" s="16"/>
-      <c r="G99" s="113"/>
+      <c r="G99" s="71"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="68">
+      <c r="A100" s="72">
         <v>11</v>
       </c>
       <c r="B100" s="21" t="s">
@@ -2621,14 +2627,14 @@
       <c r="D100" s="22"/>
       <c r="E100" s="23"/>
       <c r="F100" s="24"/>
-      <c r="G100" s="68" t="s">
+      <c r="G100" s="72" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A101" s="69"/>
-      <c r="B101" s="97" t="s">
-        <v>52</v>
+      <c r="A101" s="73"/>
+      <c r="B101" s="79" t="s">
+        <v>50</v>
       </c>
       <c r="C101" s="52" t="s">
         <v>13</v>
@@ -2640,11 +2646,11 @@
       <c r="F101" s="16">
         <v>43919</v>
       </c>
-      <c r="G101" s="69"/>
+      <c r="G101" s="73"/>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A102" s="69"/>
-      <c r="B102" s="97"/>
+      <c r="A102" s="73"/>
+      <c r="B102" s="79"/>
       <c r="C102" s="52" t="s">
         <v>14</v>
       </c>
@@ -2655,11 +2661,11 @@
       <c r="F102" s="16">
         <v>43916</v>
       </c>
-      <c r="G102" s="69"/>
+      <c r="G102" s="73"/>
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A103" s="69"/>
-      <c r="B103" s="97"/>
+      <c r="A103" s="73"/>
+      <c r="B103" s="79"/>
       <c r="C103" s="52" t="s">
         <v>15</v>
       </c>
@@ -2670,11 +2676,11 @@
       <c r="F103" s="16">
         <v>43915</v>
       </c>
-      <c r="G103" s="69"/>
+      <c r="G103" s="73"/>
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A104" s="69"/>
-      <c r="B104" s="97"/>
+      <c r="A104" s="73"/>
+      <c r="B104" s="79"/>
       <c r="C104" s="52" t="s">
         <v>16</v>
       </c>
@@ -2685,11 +2691,11 @@
       <c r="F104" s="16">
         <v>43920</v>
       </c>
-      <c r="G104" s="69"/>
+      <c r="G104" s="73"/>
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A105" s="69"/>
-      <c r="B105" s="97"/>
+      <c r="A105" s="73"/>
+      <c r="B105" s="79"/>
       <c r="C105" s="52" t="s">
         <v>17</v>
       </c>
@@ -2700,11 +2706,11 @@
       <c r="F105" s="16">
         <v>43931</v>
       </c>
-      <c r="G105" s="69"/>
+      <c r="G105" s="73"/>
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A106" s="69"/>
-      <c r="B106" s="97"/>
+      <c r="A106" s="73"/>
+      <c r="B106" s="79"/>
       <c r="C106" s="52" t="s">
         <v>18</v>
       </c>
@@ -2715,11 +2721,11 @@
       <c r="F106" s="16">
         <v>43931</v>
       </c>
-      <c r="G106" s="69"/>
+      <c r="G106" s="73"/>
     </row>
     <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A107" s="69"/>
-      <c r="B107" s="97"/>
+      <c r="A107" s="73"/>
+      <c r="B107" s="79"/>
       <c r="C107" s="52" t="s">
         <v>19</v>
       </c>
@@ -2730,10 +2736,10 @@
       <c r="F107" s="16">
         <v>43931</v>
       </c>
-      <c r="G107" s="69"/>
+      <c r="G107" s="73"/>
     </row>
     <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A108" s="69"/>
+      <c r="A108" s="73"/>
       <c r="B108" s="53" t="s">
         <v>7</v>
       </c>
@@ -2743,12 +2749,12 @@
         <v>1</v>
       </c>
       <c r="F108" s="16"/>
-      <c r="G108" s="69"/>
+      <c r="G108" s="73"/>
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A109" s="69"/>
+      <c r="A109" s="73"/>
       <c r="B109" s="53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -2758,10 +2764,10 @@
       <c r="F109" s="16">
         <v>43928</v>
       </c>
-      <c r="G109" s="69"/>
+      <c r="G109" s="73"/>
     </row>
     <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A110" s="70"/>
+      <c r="A110" s="74"/>
       <c r="B110" s="53" t="s">
         <v>8</v>
       </c>
@@ -2773,37 +2779,16 @@
       <c r="F110" s="16">
         <v>43928</v>
       </c>
-      <c r="G110" s="70"/>
+      <c r="G110" s="74"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F2" xr:uid="{60BF8AA0-547A-4AC4-BE58-D9F0611612D0}"/>
   <mergeCells count="43">
-    <mergeCell ref="G87:G93"/>
-    <mergeCell ref="G94:G99"/>
-    <mergeCell ref="G100:G110"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="A100:A110"/>
-    <mergeCell ref="B101:B107"/>
-    <mergeCell ref="A94:A99"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="A74:A80"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A20:A31"/>
-    <mergeCell ref="A32:A41"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="B21:B28"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="D9:D19"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="G8:G19"/>
+    <mergeCell ref="G32:G41"/>
+    <mergeCell ref="G42:G50"/>
+    <mergeCell ref="G51:G59"/>
     <mergeCell ref="B68:B70"/>
     <mergeCell ref="G81:G86"/>
     <mergeCell ref="G74:G80"/>
@@ -2816,11 +2801,32 @@
     <mergeCell ref="B82:B83"/>
     <mergeCell ref="D21:D31"/>
     <mergeCell ref="D33:D41"/>
-    <mergeCell ref="G3:G7"/>
-    <mergeCell ref="G8:G19"/>
-    <mergeCell ref="G32:G41"/>
-    <mergeCell ref="G42:G50"/>
-    <mergeCell ref="G51:G59"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A19"/>
+    <mergeCell ref="A20:A31"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B21:B28"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="D9:D19"/>
+    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="A51:A59"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="A74:A80"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="A100:A110"/>
+    <mergeCell ref="B101:B107"/>
+    <mergeCell ref="A94:A99"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="G87:G93"/>
+    <mergeCell ref="G94:G99"/>
+    <mergeCell ref="G100:G110"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="B95:B96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunti virtualRobot e basicRobot. Ultimato Sprint_1
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Workplan.xlsx
+++ b/DOCUMENTS/Workplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\LORI\UNIVERSITA'\Magistrale\2°Anno\II Ciclo\Ingegneria dei Sistemi Software\Waiter_Robot\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15B9DFD-FDE8-435A-8341-E1684B45A2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA41850A-750A-413C-9B8F-9986EB23DEDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
+    <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
   <si>
     <t>Sprint Goal (obiettivo)</t>
   </si>
@@ -114,21 +114,9 @@
     <t>Realizzare un pianificatore.</t>
   </si>
   <si>
-    <t>Si tratta di un componente in grado di pianificare una sequenza di comandi da attuare per raggiungere un goal.</t>
-  </si>
-  <si>
-    <t>Uno strumento consultabile per ottenere informazioni utili.</t>
-  </si>
-  <si>
-    <t>Web Application.</t>
-  </si>
-  <si>
     <t>Realizzare una base di conoscenza.</t>
   </si>
   <si>
-    <t>Sub-item</t>
-  </si>
-  <si>
     <t>4.1 Front-end</t>
   </si>
   <si>
@@ -150,18 +138,12 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Realizzazione del planner</t>
-  </si>
-  <si>
     <t>Progetto:</t>
   </si>
   <si>
     <t>Creazione di una KB della room</t>
   </si>
   <si>
-    <t>Realizzazione del basicrobot</t>
-  </si>
-  <si>
     <t>Gestione "non ottimizzata" di più clienti</t>
   </si>
   <si>
@@ -198,22 +180,64 @@
     <t>Sprint review</t>
   </si>
   <si>
-    <t>28/06?</t>
-  </si>
-  <si>
     <t>Si tratta del componente che comanda i movimenti al robot fisico.</t>
   </si>
   <si>
     <t>Robot in grado di muoversi all'interno della Tea Room</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementare </t>
-  </si>
-  <si>
-    <t>Analisi del Problema (+ creazione del modello eseguibile)</t>
-  </si>
-  <si>
     <t>Implementazione della Web Application (e della current Situation)</t>
+  </si>
+  <si>
+    <t>basicrobot</t>
+  </si>
+  <si>
+    <t>waiterwalker</t>
+  </si>
+  <si>
+    <t>Analisi del Problema</t>
+  </si>
+  <si>
+    <t>E' l'adapter verso il robot fisico.</t>
+  </si>
+  <si>
+    <t>1.1 robotSupport</t>
+  </si>
+  <si>
+    <t>Supporto alla Mappa.</t>
+  </si>
+  <si>
+    <t>Mappa della teaRoom e utils legate ad essa.</t>
+  </si>
+  <si>
+    <t>Componente in grado di pianificare i comandi da attuare per raggiungere un goal.</t>
+  </si>
+  <si>
+    <t>Supporto al planning e alla mappa</t>
+  </si>
+  <si>
+    <t>Uno strumento consultabile per ottenere informazioni utili sulla rappresentazione del dominio.</t>
+  </si>
+  <si>
+    <t>Sviluppare il waiter</t>
+  </si>
+  <si>
+    <t>Sviluppare il barman</t>
+  </si>
+  <si>
+    <t>Sviluppare la smartbell</t>
+  </si>
+  <si>
+    <t>Realizzare una Web Application per il manager</t>
+  </si>
+  <si>
+    <t>Ottimizzare il comportamento del waiter</t>
+  </si>
+  <si>
+    <t>Raffinamenti vari</t>
+  </si>
+  <si>
+    <t>CurrentSituation</t>
   </si>
 </sst>
 </file>
@@ -390,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -587,22 +611,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -612,130 +624,155 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -760,13 +797,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>6928</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>6928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>6927</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>187036</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -900,7 +937,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -986,7 +1023,7 @@
             <a:rPr lang="it-IT" sz="1100">
               <a:effectLst/>
             </a:rPr>
-            <a:t>2) Non possono essere settati come goal delle posizioni contenenti un ostacolo. Di conseguenza, non essendoci ostacoli mobili, il robot non colliderà mai.</a:t>
+            <a:t>2) Non possono essere settati come goal delle posizioni contenenti un ostacolo. Di conseguenza, non essendoci ostacoli mobili, il robot non dovrebbe collidere mai.</a:t>
           </a:r>
           <a:endParaRPr lang="it-IT">
             <a:effectLst/>
@@ -1003,12 +1040,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F927C3A-F9A7-4AA5-989C-B80BAF4C4E30}" name="Tabella2" displayName="Tabella2" ref="A1:D17" totalsRowShown="0">
-  <autoFilter ref="A1:D17" xr:uid="{6BB4EDD3-4288-4310-9006-83D3483842B4}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DB7F84C6-020F-414F-8D23-D53DBBA70C2D}" name="ID"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3F927C3A-F9A7-4AA5-989C-B80BAF4C4E30}" name="Tabella2" displayName="Tabella2" ref="A1:C18" totalsRowShown="0">
+  <autoFilter ref="A1:C18" xr:uid="{6BB4EDD3-4288-4310-9006-83D3483842B4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DB7F84C6-020F-414F-8D23-D53DBBA70C2D}" name="ID" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{EAFB3BE4-CDB0-4DA7-A1AA-6CA6AFF48949}" name="Item"/>
-    <tableColumn id="5" xr3:uid="{A945C15C-E1FA-4EDF-A97C-4EBFAE9794C3}" name="Sub-item"/>
     <tableColumn id="3" xr3:uid="{6A56A1E4-E750-4137-A2E1-96B4D8692B2B}" name="Descrizione"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1312,21 +1348,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD0328D-D609-42F7-8061-4CD2A9785B96}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
     <col min="2" max="2" width="47.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="106.33203125" customWidth="1"/>
+    <col min="3" max="3" width="106.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1334,116 +1369,146 @@
         <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="116">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="116"/>
+      <c r="B3" s="115" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="116">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="116">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="116">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="116">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="116">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="116">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="116">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="116">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="116">
+        <v>10</v>
+      </c>
+      <c r="B12" s="115" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="116">
+        <v>11</v>
+      </c>
+      <c r="B13" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="116">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="116">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="116">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="116">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="116">
         <v>16</v>
       </c>
     </row>
@@ -1458,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6357E3-4FBB-418C-9BB3-004C68F042FF}">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,21 +1536,21 @@
     <col min="3" max="3" width="79" style="57" customWidth="1"/>
     <col min="4" max="4" width="56.109375" style="57" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="59" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.77734375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
+      <c r="A1" s="94" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1499,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
@@ -1510,27 +1575,27 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="66" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D3" s="54"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="66" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
-      <c r="B4" s="90"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
@@ -1539,13 +1604,13 @@
       <c r="F4" s="11">
         <v>44002</v>
       </c>
-      <c r="G4" s="88"/>
+      <c r="G4" s="66"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="91"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
@@ -1554,13 +1619,13 @@
       <c r="F5" s="11">
         <v>44003</v>
       </c>
-      <c r="G5" s="88"/>
+      <c r="G5" s="66"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
-      <c r="B6" s="91"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="4" t="s">
@@ -1569,13 +1634,13 @@
       <c r="F6" s="11">
         <v>44004</v>
       </c>
-      <c r="G6" s="88"/>
+      <c r="G6" s="66"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
-      <c r="B7" s="92"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="s">
@@ -1584,670 +1649,700 @@
       <c r="F7" s="65">
         <v>44005</v>
       </c>
-      <c r="G7" s="88"/>
+      <c r="G7" s="66"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="81">
+      <c r="A8" s="67">
         <v>1</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="81"/>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
-      <c r="B9" s="76" t="s">
-        <v>50</v>
+      <c r="A9" s="67"/>
+      <c r="B9" s="96" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="D9" s="91"/>
+      <c r="E9" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F9" s="11">
         <v>44006</v>
       </c>
-      <c r="G9" s="81"/>
+      <c r="G9" s="67"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="81"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="97"/>
       <c r="C10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="81"/>
+        <v>52</v>
+      </c>
+      <c r="D10" s="92"/>
+      <c r="E10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>44007</v>
+      </c>
+      <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="81"/>
-      <c r="B11" s="79"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="94"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="81"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11">
+        <v>44007</v>
+      </c>
+      <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="81"/>
-      <c r="B12" s="79"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="94"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="81"/>
+        <v>33</v>
+      </c>
+      <c r="D12" s="92"/>
+      <c r="E12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11">
+        <v>44009</v>
+      </c>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" s="81"/>
-      <c r="B13" s="79"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="94"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="81"/>
+        <v>50</v>
+      </c>
+      <c r="D13" s="92"/>
+      <c r="E13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11">
+        <v>44009</v>
+      </c>
+      <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
-      <c r="B14" s="79"/>
-      <c r="C14" s="63" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="81"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="114" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="92"/>
+      <c r="E14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11">
+        <v>44009</v>
+      </c>
+      <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
-      <c r="B15" s="79"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="94"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="81"/>
+        <v>51</v>
+      </c>
+      <c r="D15" s="92"/>
+      <c r="E15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11">
+        <v>44009</v>
+      </c>
+      <c r="G15" s="67"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="81"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="98"/>
       <c r="C16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="94"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="81"/>
+        <v>32</v>
+      </c>
+      <c r="D16" s="92"/>
+      <c r="E16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
+        <v>44009</v>
+      </c>
+      <c r="G16" s="67"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="81"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="94"/>
+        <v>46</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="4"/>
-      <c r="G17" s="81"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="67"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="81"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="50" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="94"/>
+      <c r="D18" s="93"/>
       <c r="E18" s="4"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="81"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="81"/>
-      <c r="B19" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="81"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="80">
+      <c r="G18" s="67"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="84">
         <v>2</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="80"/>
+      <c r="B19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="55"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="84"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A20" s="84"/>
+      <c r="B20" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="91"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="84"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="80"/>
-      <c r="B21" s="76" t="s">
-        <v>50</v>
-      </c>
+      <c r="A21" s="84"/>
+      <c r="B21" s="97"/>
       <c r="C21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="93"/>
+        <v>37</v>
+      </c>
+      <c r="D21" s="92"/>
       <c r="E21" s="4"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="80"/>
+      <c r="G21" s="84"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
-      <c r="B22" s="79"/>
+      <c r="A22" s="84"/>
+      <c r="B22" s="97"/>
       <c r="C22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="94"/>
+        <v>12</v>
+      </c>
+      <c r="D22" s="92"/>
       <c r="E22" s="4"/>
       <c r="F22" s="16"/>
-      <c r="G22" s="80"/>
+      <c r="G22" s="84"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="80"/>
-      <c r="B23" s="79"/>
-      <c r="C23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="94"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="92"/>
       <c r="E23" s="4"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="80"/>
+      <c r="G23" s="84"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="94"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="92"/>
       <c r="E24" s="4"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="80"/>
+      <c r="G24" s="84"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
-      <c r="B25" s="79"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="94"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="92"/>
       <c r="E25" s="4"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="80"/>
+      <c r="G25" s="84"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="80"/>
-      <c r="B26" s="79"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="94"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="92"/>
       <c r="E26" s="4"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="80"/>
+      <c r="G26" s="84"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="80"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="94"/>
+      <c r="A27" s="84"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="92"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="80"/>
+      <c r="F27" s="16">
+        <v>44014</v>
+      </c>
+      <c r="G27" s="84"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="80"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="94"/>
+      <c r="A28" s="84"/>
+      <c r="B28" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="92"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="16">
-        <v>44014</v>
-      </c>
-      <c r="G28" s="80"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="84"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="80"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="94"/>
+      <c r="D29" s="93"/>
       <c r="E29" s="4"/>
       <c r="F29" s="16"/>
-      <c r="G29" s="80"/>
-    </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
-      <c r="B30" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="80"/>
+      <c r="G29" s="84"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="95">
+        <v>3</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="68"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="80"/>
-      <c r="B31" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="95"/>
+      <c r="A31" s="95"/>
+      <c r="B31" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="91"/>
       <c r="E31" s="4"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="80"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="89">
-        <v>3</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="72"/>
+      <c r="G31" s="69"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A32" s="95"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="92"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="69"/>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="89"/>
-      <c r="B33" s="76" t="s">
-        <v>50</v>
-      </c>
+      <c r="A33" s="95"/>
+      <c r="B33" s="97"/>
       <c r="C33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="93"/>
+        <v>12</v>
+      </c>
+      <c r="D33" s="92"/>
       <c r="E33" s="4"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="73"/>
+      <c r="G33" s="69"/>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A34" s="89"/>
-      <c r="B34" s="79"/>
-      <c r="C34" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="94"/>
+      <c r="A34" s="95"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="92"/>
       <c r="E34" s="4"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="73"/>
+      <c r="G34" s="69"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="89"/>
-      <c r="B35" s="79"/>
-      <c r="C35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="94"/>
+      <c r="A35" s="95"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="92"/>
       <c r="E35" s="4"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="73"/>
+      <c r="G35" s="69"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="89"/>
-      <c r="B36" s="79"/>
-      <c r="C36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="94"/>
+      <c r="A36" s="95"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="92"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="73"/>
+      <c r="F36" s="16">
+        <v>44018</v>
+      </c>
+      <c r="G36" s="69"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="89"/>
-      <c r="B37" s="79"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="94"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="64"/>
+      <c r="D37" s="92"/>
       <c r="E37" s="4"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="73"/>
+      <c r="G37" s="69"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="89"/>
-      <c r="B38" s="77"/>
-      <c r="C38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="94"/>
+      <c r="A38" s="95"/>
+      <c r="B38" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="93"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="16">
-        <v>44018</v>
-      </c>
-      <c r="G38" s="73"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="89"/>
-      <c r="B39" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="63"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="73"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="70"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="102">
+        <v>4</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="71"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="89"/>
-      <c r="B40" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="64"/>
-      <c r="D40" s="94"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
       <c r="E40" s="4"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="73"/>
+      <c r="G40" s="72"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="89"/>
-      <c r="B41" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="95"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="4"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="74"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="82">
-        <v>4</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="108"/>
+      <c r="G41" s="72"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A42" s="102"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="72"/>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="82"/>
-      <c r="B43" s="75" t="s">
-        <v>50</v>
-      </c>
+      <c r="A43" s="102"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="4"/>
       <c r="F43" s="16"/>
-      <c r="G43" s="109"/>
+      <c r="G43" s="72"/>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="82"/>
-      <c r="B44" s="75"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="A44" s="102"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
       <c r="E44" s="4"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="109"/>
+      <c r="F44" s="16">
+        <v>44022</v>
+      </c>
+      <c r="G44" s="72"/>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="82"/>
-      <c r="B45" s="75"/>
+      <c r="A45" s="102"/>
+      <c r="B45" s="50" t="s">
+        <v>46</v>
+      </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="4"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="109"/>
+      <c r="G45" s="72"/>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="82"/>
-      <c r="B46" s="75"/>
+      <c r="A46" s="102"/>
+      <c r="B46" s="50" t="s">
+        <v>8</v>
+      </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="4"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="109"/>
-    </row>
-    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A47" s="82"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="16">
-        <v>44022</v>
-      </c>
-      <c r="G47" s="109"/>
+      <c r="G46" s="73"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="103">
+        <v>5</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="30"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="74"/>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="82"/>
-      <c r="B48" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="2"/>
+      <c r="A48" s="103"/>
+      <c r="B48" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="4"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="109"/>
+      <c r="G48" s="75"/>
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="82"/>
-      <c r="B49" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="2"/>
+      <c r="A49" s="103"/>
+      <c r="B49" s="77"/>
+      <c r="C49" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D49" s="2"/>
       <c r="E49" s="4"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="109"/>
+      <c r="G49" s="75"/>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" s="82"/>
-      <c r="B50" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="2"/>
+      <c r="A50" s="103"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="4"/>
       <c r="F50" s="16"/>
-      <c r="G50" s="110"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="83">
-        <v>5</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" s="30"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="111"/>
+      <c r="G50" s="75"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A51" s="103"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="75"/>
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="83"/>
-      <c r="B52" s="75" t="s">
-        <v>50</v>
-      </c>
+      <c r="A52" s="103"/>
+      <c r="B52" s="77"/>
       <c r="C52" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="112"/>
+      <c r="F52" s="16">
+        <v>44026</v>
+      </c>
+      <c r="G52" s="75"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="83"/>
-      <c r="B53" s="75"/>
-      <c r="C53" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="A53" s="103"/>
+      <c r="B53" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="5"/>
       <c r="D53" s="2"/>
       <c r="E53" s="4"/>
       <c r="F53" s="16"/>
-      <c r="G53" s="112"/>
+      <c r="G53" s="75"/>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="83"/>
-      <c r="B54" s="75"/>
-      <c r="C54" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A54" s="103"/>
+      <c r="B54" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="5"/>
       <c r="D54" s="2"/>
       <c r="E54" s="4"/>
       <c r="F54" s="16"/>
-      <c r="G54" s="112"/>
-    </row>
-    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="83"/>
-      <c r="B55" s="75"/>
-      <c r="C55" s="1" t="s">
+      <c r="G54" s="76"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="104">
+        <v>6</v>
+      </c>
+      <c r="B55" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="112"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="85"/>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="83"/>
-      <c r="B56" s="75"/>
-      <c r="C56" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A56" s="104"/>
+      <c r="B56" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="16">
-        <v>44026</v>
-      </c>
-      <c r="G56" s="112"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="86"/>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="83"/>
-      <c r="B57" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="5"/>
+      <c r="A57" s="104"/>
+      <c r="B57" s="77"/>
+      <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="112"/>
+      <c r="G57" s="86"/>
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A58" s="83"/>
-      <c r="B58" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C58" s="5"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="77"/>
+      <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="4"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="112"/>
+      <c r="G58" s="86"/>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="83"/>
+      <c r="A59" s="104"/>
       <c r="B59" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="4"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="113"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="84">
+      <c r="G59" s="86"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A60" s="104"/>
+      <c r="B60" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="87"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="105">
         <v>6</v>
       </c>
-      <c r="B60" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C60" s="49" t="s">
+      <c r="B61" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="88"/>
+    </row>
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A62" s="105"/>
+      <c r="B62" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D60" s="49"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="102"/>
-    </row>
-    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" s="84"/>
-      <c r="B61" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="103"/>
-    </row>
-    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A62" s="84"/>
-      <c r="B62" s="75"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="4"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="103"/>
+      <c r="G62" s="89"/>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="84"/>
-      <c r="B63" s="75"/>
+      <c r="A63" s="105"/>
+      <c r="B63" s="77"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="4"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="103"/>
+      <c r="G63" s="89"/>
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" s="84"/>
-      <c r="B64" s="50" t="s">
-        <v>7</v>
-      </c>
+      <c r="A64" s="105"/>
+      <c r="B64" s="77"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="4"/>
       <c r="F64" s="16"/>
-      <c r="G64" s="103"/>
+      <c r="G64" s="89"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="84"/>
+      <c r="A65" s="105"/>
       <c r="B65" s="50" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="4"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="103"/>
+      <c r="G65" s="89"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="84"/>
+      <c r="A66" s="105"/>
       <c r="B66" s="50" t="s">
         <v>8</v>
       </c>
@@ -2255,578 +2350,492 @@
       <c r="D66" s="2"/>
       <c r="E66" s="4"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="104"/>
+      <c r="G66" s="90"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="85">
-        <v>6</v>
-      </c>
-      <c r="B67" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="105"/>
+      <c r="A67" s="106">
+        <v>7</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="81"/>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A68" s="85"/>
-      <c r="B68" s="75" t="s">
-        <v>50</v>
+      <c r="A68" s="106"/>
+      <c r="B68" s="77" t="s">
+        <v>44</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="4"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="106"/>
+      <c r="G68" s="82"/>
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="85"/>
-      <c r="B69" s="75"/>
+      <c r="A69" s="106"/>
+      <c r="B69" s="77"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="4"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="106"/>
+      <c r="G69" s="82"/>
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A70" s="85"/>
-      <c r="B70" s="75"/>
+      <c r="A70" s="106"/>
+      <c r="B70" s="77"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="4"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="106"/>
+      <c r="G70" s="82"/>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A71" s="85"/>
+      <c r="A71" s="106"/>
       <c r="B71" s="50" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="4"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="106"/>
+      <c r="G71" s="82"/>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="85"/>
+      <c r="A72" s="106"/>
       <c r="B72" s="50" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="4"/>
       <c r="F72" s="16"/>
-      <c r="G72" s="106"/>
-    </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A73" s="85"/>
-      <c r="B73" s="50" t="s">
+      <c r="G72" s="83"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="107">
         <v>8</v>
       </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="107"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="86">
-        <v>7</v>
-      </c>
-      <c r="B74" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="41"/>
-      <c r="G74" s="99"/>
+      <c r="B73" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="45"/>
+      <c r="G73" s="78"/>
+    </row>
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A74" s="107"/>
+      <c r="B74" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="79"/>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A75" s="86"/>
-      <c r="B75" s="75" t="s">
-        <v>50</v>
-      </c>
+      <c r="A75" s="107"/>
+      <c r="B75" s="77"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="4"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="100"/>
+      <c r="G75" s="79"/>
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A76" s="86"/>
-      <c r="B76" s="75"/>
+      <c r="A76" s="107"/>
+      <c r="B76" s="50" t="s">
+        <v>7</v>
+      </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="4"/>
       <c r="F76" s="16"/>
-      <c r="G76" s="100"/>
+      <c r="G76" s="79"/>
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A77" s="86"/>
-      <c r="B77" s="75"/>
+      <c r="A77" s="107"/>
+      <c r="B77" s="50" t="s">
+        <v>46</v>
+      </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="4"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="100"/>
+      <c r="G77" s="79"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A78" s="86"/>
+      <c r="A78" s="107"/>
       <c r="B78" s="50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="4"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="100"/>
-    </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A79" s="86"/>
-      <c r="B79" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="100"/>
+      <c r="G78" s="80"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="67">
+        <v>9</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="108"/>
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A80" s="86"/>
-      <c r="B80" s="50" t="s">
-        <v>8</v>
+      <c r="A80" s="67"/>
+      <c r="B80" s="77" t="s">
+        <v>44</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="4"/>
       <c r="F80" s="16"/>
-      <c r="G80" s="101"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="78">
-        <v>8</v>
-      </c>
-      <c r="B81" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="43"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="44"/>
-      <c r="F81" s="45"/>
-      <c r="G81" s="96"/>
+      <c r="G80" s="109"/>
+    </row>
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A81" s="67"/>
+      <c r="B81" s="77"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="109"/>
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A82" s="78"/>
-      <c r="B82" s="75" t="s">
-        <v>50</v>
-      </c>
+      <c r="A82" s="67"/>
+      <c r="B82" s="77"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="4"/>
       <c r="F82" s="16"/>
-      <c r="G82" s="97"/>
+      <c r="G82" s="109"/>
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A83" s="78"/>
-      <c r="B83" s="75"/>
+      <c r="A83" s="67"/>
+      <c r="B83" s="50" t="s">
+        <v>7</v>
+      </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="4"/>
       <c r="F83" s="16"/>
-      <c r="G83" s="97"/>
+      <c r="G83" s="109"/>
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A84" s="78"/>
+      <c r="A84" s="67"/>
       <c r="B84" s="50" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="4"/>
       <c r="F84" s="16"/>
-      <c r="G84" s="97"/>
+      <c r="G84" s="109"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A85" s="78"/>
+      <c r="A85" s="67"/>
       <c r="B85" s="50" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="4"/>
       <c r="F85" s="16"/>
-      <c r="G85" s="97"/>
-    </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A86" s="78"/>
-      <c r="B86" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="98"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="81">
-        <v>9</v>
-      </c>
-      <c r="B87" s="12" t="s">
+      <c r="G85" s="110"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="84">
+        <v>10</v>
+      </c>
+      <c r="B86" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="15"/>
-      <c r="G87" s="66"/>
+      <c r="C86" s="47"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="111"/>
+    </row>
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A87" s="84"/>
+      <c r="B87" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="112"/>
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A88" s="81"/>
-      <c r="B88" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="A88" s="84"/>
+      <c r="B88" s="98"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
       <c r="E88" s="4"/>
       <c r="F88" s="16"/>
-      <c r="G88" s="67"/>
+      <c r="G88" s="112"/>
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A89" s="81"/>
-      <c r="B89" s="75"/>
+      <c r="A89" s="84"/>
+      <c r="B89" s="50" t="s">
+        <v>7</v>
+      </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="4"/>
       <c r="F89" s="16"/>
-      <c r="G89" s="67"/>
+      <c r="G89" s="112"/>
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A90" s="81"/>
-      <c r="B90" s="75"/>
+      <c r="A90" s="84"/>
+      <c r="B90" s="50" t="s">
+        <v>46</v>
+      </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="4"/>
       <c r="F90" s="16"/>
-      <c r="G90" s="67"/>
+      <c r="G90" s="112"/>
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="81"/>
+      <c r="A91" s="84"/>
       <c r="B91" s="50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="4"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="67"/>
-    </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A92" s="81"/>
-      <c r="B92" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="16"/>
-      <c r="G92" s="67"/>
+      <c r="G91" s="113"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="68">
+        <v>11</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="22"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="68" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A93" s="81"/>
-      <c r="B93" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="16"/>
-      <c r="G93" s="68"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="80">
-        <v>10</v>
-      </c>
-      <c r="B94" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C94" s="47"/>
-      <c r="D94" s="47"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="20"/>
+      <c r="A93" s="69"/>
+      <c r="B93" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D93" s="52"/>
+      <c r="E93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" s="16">
+        <v>43919</v>
+      </c>
+      <c r="G93" s="69"/>
+    </row>
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A94" s="69"/>
+      <c r="B94" s="97"/>
+      <c r="C94" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" s="52"/>
+      <c r="E94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="16">
+        <v>43916</v>
+      </c>
       <c r="G94" s="69"/>
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A95" s="80"/>
-      <c r="B95" s="76" t="s">
-        <v>50</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="70"/>
+      <c r="A95" s="69"/>
+      <c r="B95" s="97"/>
+      <c r="C95" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="52"/>
+      <c r="E95" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="16">
+        <v>43915</v>
+      </c>
+      <c r="G95" s="69"/>
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A96" s="80"/>
-      <c r="B96" s="77"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="70"/>
+      <c r="A96" s="69"/>
+      <c r="B96" s="97"/>
+      <c r="C96" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="52"/>
+      <c r="E96" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F96" s="16">
+        <v>43920</v>
+      </c>
+      <c r="G96" s="69"/>
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A97" s="80"/>
-      <c r="B97" s="50" t="s">
+      <c r="A97" s="69"/>
+      <c r="B97" s="97"/>
+      <c r="C97" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D97" s="52"/>
+      <c r="E97" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" s="16">
+        <v>43931</v>
+      </c>
+      <c r="G97" s="69"/>
+    </row>
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A98" s="69"/>
+      <c r="B98" s="97"/>
+      <c r="C98" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98" s="52"/>
+      <c r="E98" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F98" s="16">
+        <v>43931</v>
+      </c>
+      <c r="G98" s="69"/>
+    </row>
+    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A99" s="69"/>
+      <c r="B99" s="97"/>
+      <c r="C99" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D99" s="52"/>
+      <c r="E99" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F99" s="16">
+        <v>43931</v>
+      </c>
+      <c r="G99" s="69"/>
+    </row>
+    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A100" s="69"/>
+      <c r="B100" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="70"/>
-    </row>
-    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A98" s="80"/>
-      <c r="B98" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="16"/>
-      <c r="G98" s="70"/>
-    </row>
-    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A99" s="80"/>
-      <c r="B99" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="71"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="72">
-        <v>11</v>
-      </c>
-      <c r="B100" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C100" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" s="22"/>
-      <c r="E100" s="23"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="72" t="s">
-        <v>10</v>
-      </c>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F100" s="16"/>
+      <c r="G100" s="69"/>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A101" s="73"/>
-      <c r="B101" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="C101" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D101" s="52"/>
+      <c r="A101" s="69"/>
+      <c r="B101" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
       <c r="E101" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F101" s="16">
-        <v>43919</v>
-      </c>
-      <c r="G101" s="73"/>
+        <v>43928</v>
+      </c>
+      <c r="G101" s="69"/>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A102" s="73"/>
-      <c r="B102" s="79"/>
-      <c r="C102" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" s="52"/>
+      <c r="A102" s="70"/>
+      <c r="B102" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
       <c r="E102" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F102" s="16">
-        <v>43916</v>
-      </c>
-      <c r="G102" s="73"/>
-    </row>
-    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A103" s="73"/>
-      <c r="B103" s="79"/>
-      <c r="C103" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="D103" s="52"/>
-      <c r="E103" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F103" s="16">
-        <v>43915</v>
-      </c>
-      <c r="G103" s="73"/>
-    </row>
-    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A104" s="73"/>
-      <c r="B104" s="79"/>
-      <c r="C104" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D104" s="52"/>
-      <c r="E104" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F104" s="16">
-        <v>43920</v>
-      </c>
-      <c r="G104" s="73"/>
-    </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A105" s="73"/>
-      <c r="B105" s="79"/>
-      <c r="C105" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D105" s="52"/>
-      <c r="E105" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F105" s="16">
-        <v>43931</v>
-      </c>
-      <c r="G105" s="73"/>
-    </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A106" s="73"/>
-      <c r="B106" s="79"/>
-      <c r="C106" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="D106" s="52"/>
-      <c r="E106" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F106" s="16">
-        <v>43931</v>
-      </c>
-      <c r="G106" s="73"/>
-    </row>
-    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A107" s="73"/>
-      <c r="B107" s="79"/>
-      <c r="C107" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="D107" s="52"/>
-      <c r="E107" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F107" s="16">
-        <v>43931</v>
-      </c>
-      <c r="G107" s="73"/>
-    </row>
-    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A108" s="73"/>
-      <c r="B108" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F108" s="16"/>
-      <c r="G108" s="73"/>
-    </row>
-    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A109" s="73"/>
-      <c r="B109" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F109" s="16">
         <v>43928</v>
       </c>
-      <c r="G109" s="73"/>
-    </row>
-    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A110" s="74"/>
-      <c r="B110" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F110" s="16">
-        <v>43928</v>
-      </c>
-      <c r="G110" s="74"/>
+      <c r="G102" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F2" xr:uid="{60BF8AA0-547A-4AC4-BE58-D9F0611612D0}"/>
   <mergeCells count="43">
-    <mergeCell ref="G3:G7"/>
-    <mergeCell ref="G8:G19"/>
-    <mergeCell ref="G32:G41"/>
-    <mergeCell ref="G42:G50"/>
-    <mergeCell ref="G51:G59"/>
+    <mergeCell ref="G79:G85"/>
+    <mergeCell ref="G86:G91"/>
+    <mergeCell ref="G92:G102"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="A73:A78"/>
     <mergeCell ref="B68:B70"/>
-    <mergeCell ref="G81:G86"/>
-    <mergeCell ref="G74:G80"/>
-    <mergeCell ref="G20:G31"/>
-    <mergeCell ref="G60:G66"/>
-    <mergeCell ref="G67:G73"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="D21:D31"/>
-    <mergeCell ref="D33:D41"/>
+    <mergeCell ref="A92:A102"/>
+    <mergeCell ref="B93:B99"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="A47:A54"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="A67:A72"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A20:A31"/>
-    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="A30:A38"/>
     <mergeCell ref="B9:B16"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="B21:B28"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B20:B27"/>
     <mergeCell ref="B4:B7"/>
-    <mergeCell ref="D9:D19"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="A51:A59"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="A74:A80"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="A100:A110"/>
-    <mergeCell ref="B101:B107"/>
-    <mergeCell ref="A94:A99"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="G87:G93"/>
-    <mergeCell ref="G94:G99"/>
-    <mergeCell ref="G100:G110"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="G73:G78"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="G19:G29"/>
+    <mergeCell ref="G55:G60"/>
+    <mergeCell ref="G61:G66"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="D20:D29"/>
+    <mergeCell ref="D31:D38"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="G8:G18"/>
+    <mergeCell ref="G30:G38"/>
+    <mergeCell ref="G39:G46"/>
+    <mergeCell ref="G47:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementato maxStayTime observer. Quasi ultimato Sprint2
</commit_message>
<xml_diff>
--- a/DOCUMENTS/Workplan.xlsx
+++ b/DOCUMENTS/Workplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\LORI\UNIVERSITA'\Magistrale\2°Anno\II Ciclo\Ingegneria dei Sistemi Software\Waiter_Robot\DOCUMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA41850A-750A-413C-9B8F-9986EB23DEDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4364F8A-1826-43C3-B9A9-082F64878B41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
+    <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" activeTab="1" xr2:uid="{A454F38D-EC97-4B78-83EB-CF946ED58C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="69">
   <si>
     <t>Sprint Goal (obiettivo)</t>
   </si>
@@ -237,14 +237,20 @@
     <t>Raffinamenti vari</t>
   </si>
   <si>
-    <t>CurrentSituation</t>
+    <t>Affrontare la problematica MaxStayTime</t>
+  </si>
+  <si>
+    <t>Affrontare la problematica CurrentSituation</t>
+  </si>
+  <si>
+    <t>Implementare il MaxStayTime Countdown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +286,14 @@
       <color theme="1"/>
       <name val="Segoe UI Symbol"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -611,10 +625,31 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -624,66 +659,57 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -695,74 +721,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,15 +810,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>6928</xdr:colOff>
+      <xdr:colOff>6929</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>6928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>6927</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3836895</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>187036</xdr:rowOff>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -819,8 +833,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7557655" y="3671455"/>
-          <a:ext cx="3851563" cy="2119745"/>
+          <a:off x="7555211" y="3592810"/>
+          <a:ext cx="3829966" cy="1866696"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -888,12 +902,26 @@
             </a:rPr>
             <a:t>Al barman, di conseguenza, sarà richiesto di lavorare alla preparazione di un ordine alla volta. </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3) Il tempo di preparazione di un ordine è sempre lo stesso, a prescindere da cosa è stato ordinato.</a:t>
+          </a:r>
           <a:endParaRPr lang="it-IT" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="it-IT" sz="1100"/>
-            <a:t>3) </a:t>
+            <a:t>4) </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="it-IT" sz="1100">
@@ -907,20 +935,6 @@
             </a:rPr>
             <a:t>I task del waiter non sono interrompibili.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="it-IT" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>4) Il waiter conosce già la mappa della stanza.</a:t>
-          </a:r>
           <a:endParaRPr lang="it-IT" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -932,13 +946,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>6929</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>8964</xdr:rowOff>
+      <xdr:rowOff>8965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>179296</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -953,8 +967,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7555211" y="1479176"/>
-          <a:ext cx="3838931" cy="2115672"/>
+          <a:off x="7555211" y="1479177"/>
+          <a:ext cx="3838931" cy="1918448"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1350,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD0328D-D609-42F7-8061-4CD2A9785B96}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,7 +1387,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="116">
+      <c r="A2" s="68">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1384,8 +1398,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="116"/>
-      <c r="B3" s="115" t="s">
+      <c r="A3" s="68"/>
+      <c r="B3" s="67" t="s">
         <v>54</v>
       </c>
       <c r="C3" t="s">
@@ -1393,7 +1407,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="116">
+      <c r="A4" s="68">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1404,7 +1418,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="116">
+      <c r="A5" s="68">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1415,7 +1429,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="116">
+      <c r="A6" s="68">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1426,89 +1440,92 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="116">
+      <c r="A7" s="68">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="68">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="116">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="68">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="116">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="68">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="116">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="116">
+      <c r="A11" s="68">
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="68">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="116">
-        <v>10</v>
-      </c>
-      <c r="B12" s="115" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="68">
+        <v>11</v>
+      </c>
+      <c r="B13" s="67" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="116">
-        <v>11</v>
-      </c>
-      <c r="B13" s="115" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="68">
+        <v>12</v>
+      </c>
+      <c r="B14" s="67" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="116">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="68">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="116">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="68">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="116">
-        <v>14</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="116">
+      <c r="A17" s="68">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="116">
+      <c r="A18" s="68">
         <v>16</v>
       </c>
     </row>
@@ -1525,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6357E3-4FBB-418C-9BB3-004C68F042FF}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1542,15 +1559,15 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1575,7 +1592,7 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="90" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1587,13 +1604,13 @@
       <c r="D3" s="54"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="90" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
-      <c r="B4" s="99"/>
+      <c r="A4" s="90"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1604,11 +1621,11 @@
       <c r="F4" s="11">
         <v>44002</v>
       </c>
-      <c r="G4" s="66"/>
+      <c r="G4" s="90"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="100"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1619,11 +1636,11 @@
       <c r="F5" s="11">
         <v>44003</v>
       </c>
-      <c r="G5" s="66"/>
+      <c r="G5" s="90"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
-      <c r="B6" s="100"/>
+      <c r="A6" s="90"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="2" t="s">
         <v>39</v>
       </c>
@@ -1634,11 +1651,11 @@
       <c r="F6" s="11">
         <v>44004</v>
       </c>
-      <c r="G6" s="66"/>
+      <c r="G6" s="90"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="66"/>
-      <c r="B7" s="101"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
@@ -1649,10 +1666,10 @@
       <c r="F7" s="65">
         <v>44005</v>
       </c>
-      <c r="G7" s="66"/>
+      <c r="G7" s="90"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="67">
+      <c r="A8" s="84">
         <v>1</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1664,154 +1681,154 @@
       <c r="D8" s="13"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="67"/>
+      <c r="G8" s="84" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
-      <c r="B9" s="96" t="s">
+      <c r="A9" s="84"/>
+      <c r="B9" s="79" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="91"/>
+      <c r="D9" s="95"/>
       <c r="E9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="11">
         <v>44006</v>
       </c>
-      <c r="G9" s="67"/>
+      <c r="G9" s="84"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="97"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="92"/>
+      <c r="D10" s="96"/>
       <c r="E10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="11">
         <v>44007</v>
       </c>
-      <c r="G10" s="67"/>
+      <c r="G10" s="84"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
-      <c r="B11" s="97"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="92"/>
+      <c r="D11" s="96"/>
       <c r="E11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="11">
         <v>44007</v>
       </c>
-      <c r="G11" s="67"/>
+      <c r="G11" s="84"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="97"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="92"/>
+      <c r="D12" s="96"/>
       <c r="E12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="11">
-        <v>44009</v>
-      </c>
-      <c r="G12" s="67"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="84"/>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
-      <c r="B13" s="97"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="92"/>
+      <c r="D13" s="96"/>
       <c r="E13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="11">
         <v>44009</v>
       </c>
-      <c r="G13" s="67"/>
+      <c r="G13" s="84"/>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
-      <c r="B14" s="97"/>
-      <c r="C14" s="114" t="s">
+      <c r="A14" s="84"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="92"/>
+      <c r="D14" s="96"/>
       <c r="E14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="11">
         <v>44009</v>
       </c>
-      <c r="G14" s="67"/>
+      <c r="G14" s="84"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
-      <c r="B15" s="97"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="92"/>
+      <c r="D15" s="96"/>
       <c r="E15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="11">
         <v>44009</v>
       </c>
-      <c r="G15" s="67"/>
+      <c r="G15" s="84"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="98"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="92"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="11">
         <v>44009</v>
       </c>
-      <c r="G16" s="67"/>
+      <c r="G16" s="84"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="67"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="50" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="92"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="4"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="67"/>
+      <c r="G17" s="84"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="93"/>
+      <c r="D18" s="97"/>
       <c r="E18" s="4"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="67"/>
+      <c r="G18" s="84"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="84">
+      <c r="A19" s="83">
         <v>2</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -1823,120 +1840,130 @@
       <c r="D19" s="55"/>
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="84"/>
+      <c r="G19" s="83"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="84"/>
-      <c r="B20" s="96" t="s">
+      <c r="A20" s="83"/>
+      <c r="B20" s="79" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="91"/>
+      <c r="D20" s="95"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="84"/>
+      <c r="F20" s="16">
+        <v>44010</v>
+      </c>
+      <c r="G20" s="83"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="84"/>
-      <c r="B21" s="97"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="92"/>
+      <c r="D21" s="96"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="84"/>
+      <c r="F21" s="16">
+        <v>44012</v>
+      </c>
+      <c r="G21" s="83"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="84"/>
-      <c r="B22" s="97"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="92"/>
+      <c r="D22" s="96"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="84"/>
+      <c r="F22" s="16">
+        <v>44012</v>
+      </c>
+      <c r="G22" s="83"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="84"/>
-      <c r="B23" s="97"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="92"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="4"/>
       <c r="F23" s="16"/>
-      <c r="G23" s="84"/>
+      <c r="G23" s="83"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="84"/>
-      <c r="B24" s="97"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="92"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="84"/>
+      <c r="F24" s="16">
+        <v>44013</v>
+      </c>
+      <c r="G24" s="83"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="84"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="92"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="96"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="84"/>
+      <c r="F25" s="16">
+        <v>44015</v>
+      </c>
+      <c r="G25" s="83"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="84"/>
-      <c r="B26" s="97"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="92"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="82"/>
+      <c r="C26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="96"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="84"/>
+      <c r="F26" s="16">
+        <v>44016</v>
+      </c>
+      <c r="G26" s="83"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="98"/>
-      <c r="C27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="92"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="80"/>
+      <c r="D27" s="96"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="16">
-        <v>44014</v>
-      </c>
-      <c r="G27" s="84"/>
+      <c r="G27" s="83"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="84"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="60" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="92"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="4"/>
       <c r="F28" s="16"/>
-      <c r="G28" s="84"/>
+      <c r="G28" s="83"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="84"/>
+      <c r="A29" s="83"/>
       <c r="B29" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="93"/>
+      <c r="D29" s="97"/>
       <c r="E29" s="4"/>
       <c r="F29" s="16"/>
-      <c r="G29" s="84"/>
+      <c r="G29" s="83"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="95">
+      <c r="A30" s="91">
         <v>3</v>
       </c>
       <c r="B30" s="21" t="s">
@@ -1948,100 +1975,100 @@
       <c r="D30" s="22"/>
       <c r="E30" s="23"/>
       <c r="F30" s="24"/>
-      <c r="G30" s="68"/>
+      <c r="G30" s="75"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="95"/>
-      <c r="B31" s="96" t="s">
+      <c r="A31" s="91"/>
+      <c r="B31" s="79" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="91"/>
+      <c r="D31" s="95"/>
       <c r="E31" s="4"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="69"/>
+      <c r="G31" s="76"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A32" s="95"/>
-      <c r="B32" s="97"/>
+      <c r="A32" s="91"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="92"/>
+      <c r="D32" s="96"/>
       <c r="E32" s="4"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="69"/>
+      <c r="G32" s="76"/>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="95"/>
-      <c r="B33" s="97"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="92"/>
+      <c r="D33" s="96"/>
       <c r="E33" s="4"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="69"/>
+      <c r="G33" s="76"/>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A34" s="95"/>
-      <c r="B34" s="97"/>
+      <c r="A34" s="91"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="92"/>
+      <c r="D34" s="96"/>
       <c r="E34" s="4"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="69"/>
+      <c r="G34" s="76"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="95"/>
-      <c r="B35" s="97"/>
+      <c r="A35" s="91"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="92"/>
+      <c r="D35" s="96"/>
       <c r="E35" s="4"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="69"/>
+      <c r="G35" s="76"/>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="95"/>
-      <c r="B36" s="98"/>
+      <c r="A36" s="91"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="92"/>
+      <c r="D36" s="96"/>
       <c r="E36" s="4"/>
       <c r="F36" s="16">
         <v>44018</v>
       </c>
-      <c r="G36" s="69"/>
+      <c r="G36" s="76"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="95"/>
+      <c r="A37" s="91"/>
       <c r="B37" s="50" t="s">
         <v>46</v>
       </c>
       <c r="C37" s="64"/>
-      <c r="D37" s="92"/>
+      <c r="D37" s="96"/>
       <c r="E37" s="4"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="69"/>
+      <c r="G37" s="76"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="95"/>
+      <c r="A38" s="91"/>
       <c r="B38" s="50" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="93"/>
+      <c r="D38" s="97"/>
       <c r="E38" s="4"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="70"/>
+      <c r="G38" s="77"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="102">
+      <c r="A39" s="85">
         <v>4</v>
       </c>
       <c r="B39" s="25" t="s">
@@ -2053,59 +2080,59 @@
       <c r="D39" s="26"/>
       <c r="E39" s="27"/>
       <c r="F39" s="28"/>
-      <c r="G39" s="71"/>
+      <c r="G39" s="110"/>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="102"/>
-      <c r="B40" s="77" t="s">
+      <c r="A40" s="85"/>
+      <c r="B40" s="78" t="s">
         <v>44</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="4"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="72"/>
+      <c r="G40" s="111"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="102"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="78"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="4"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="72"/>
+      <c r="G41" s="111"/>
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="102"/>
-      <c r="B42" s="77"/>
+      <c r="A42" s="85"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="4"/>
       <c r="F42" s="16"/>
-      <c r="G42" s="72"/>
+      <c r="G42" s="111"/>
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="102"/>
-      <c r="B43" s="77"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="78"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="4"/>
       <c r="F43" s="16"/>
-      <c r="G43" s="72"/>
+      <c r="G43" s="111"/>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="102"/>
-      <c r="B44" s="77"/>
+      <c r="A44" s="85"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="61"/>
       <c r="D44" s="61"/>
       <c r="E44" s="4"/>
       <c r="F44" s="16">
         <v>44022</v>
       </c>
-      <c r="G44" s="72"/>
+      <c r="G44" s="111"/>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="102"/>
+      <c r="A45" s="85"/>
       <c r="B45" s="50" t="s">
         <v>46</v>
       </c>
@@ -2113,10 +2140,10 @@
       <c r="D45" s="2"/>
       <c r="E45" s="4"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="72"/>
+      <c r="G45" s="111"/>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="102"/>
+      <c r="A46" s="85"/>
       <c r="B46" s="50" t="s">
         <v>8</v>
       </c>
@@ -2124,10 +2151,10 @@
       <c r="D46" s="2"/>
       <c r="E46" s="4"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="73"/>
+      <c r="G46" s="112"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="103">
+      <c r="A47" s="86">
         <v>5</v>
       </c>
       <c r="B47" s="29" t="s">
@@ -2139,11 +2166,11 @@
       <c r="D47" s="30"/>
       <c r="E47" s="31"/>
       <c r="F47" s="32"/>
-      <c r="G47" s="74"/>
+      <c r="G47" s="113"/>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A48" s="103"/>
-      <c r="B48" s="77" t="s">
+      <c r="A48" s="86"/>
+      <c r="B48" s="78" t="s">
         <v>44</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -2152,44 +2179,44 @@
       <c r="D48" s="2"/>
       <c r="E48" s="4"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="75"/>
+      <c r="G48" s="114"/>
     </row>
     <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A49" s="103"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="86"/>
+      <c r="B49" s="78"/>
       <c r="C49" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="4"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="75"/>
+      <c r="G49" s="114"/>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A50" s="103"/>
-      <c r="B50" s="77"/>
+      <c r="A50" s="86"/>
+      <c r="B50" s="78"/>
       <c r="C50" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="4"/>
       <c r="F50" s="16"/>
-      <c r="G50" s="75"/>
+      <c r="G50" s="114"/>
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A51" s="103"/>
-      <c r="B51" s="77"/>
+      <c r="A51" s="86"/>
+      <c r="B51" s="78"/>
       <c r="C51" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="4"/>
       <c r="F51" s="16"/>
-      <c r="G51" s="75"/>
+      <c r="G51" s="114"/>
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="103"/>
-      <c r="B52" s="77"/>
+      <c r="A52" s="86"/>
+      <c r="B52" s="78"/>
       <c r="C52" s="2" t="s">
         <v>32</v>
       </c>
@@ -2198,10 +2225,10 @@
       <c r="F52" s="16">
         <v>44026</v>
       </c>
-      <c r="G52" s="75"/>
+      <c r="G52" s="114"/>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="103"/>
+      <c r="A53" s="86"/>
       <c r="B53" s="50" t="s">
         <v>46</v>
       </c>
@@ -2209,10 +2236,10 @@
       <c r="D53" s="2"/>
       <c r="E53" s="4"/>
       <c r="F53" s="16"/>
-      <c r="G53" s="75"/>
+      <c r="G53" s="114"/>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="103"/>
+      <c r="A54" s="86"/>
       <c r="B54" s="50" t="s">
         <v>8</v>
       </c>
@@ -2220,10 +2247,10 @@
       <c r="D54" s="2"/>
       <c r="E54" s="4"/>
       <c r="F54" s="16"/>
-      <c r="G54" s="76"/>
+      <c r="G54" s="115"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="104">
+      <c r="A55" s="87">
         <v>6</v>
       </c>
       <c r="B55" s="48" t="s">
@@ -2235,39 +2262,39 @@
       <c r="D55" s="49"/>
       <c r="E55" s="33"/>
       <c r="F55" s="34"/>
-      <c r="G55" s="85"/>
+      <c r="G55" s="104"/>
     </row>
     <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="104"/>
-      <c r="B56" s="77" t="s">
+      <c r="A56" s="87"/>
+      <c r="B56" s="78" t="s">
         <v>44</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="4"/>
       <c r="F56" s="16"/>
-      <c r="G56" s="86"/>
+      <c r="G56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A57" s="104"/>
-      <c r="B57" s="77"/>
+      <c r="A57" s="87"/>
+      <c r="B57" s="78"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="4"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="86"/>
+      <c r="G57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A58" s="104"/>
-      <c r="B58" s="77"/>
+      <c r="A58" s="87"/>
+      <c r="B58" s="78"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="4"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="86"/>
+      <c r="G58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A59" s="104"/>
+      <c r="A59" s="87"/>
       <c r="B59" s="50" t="s">
         <v>46</v>
       </c>
@@ -2275,10 +2302,10 @@
       <c r="D59" s="2"/>
       <c r="E59" s="4"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="86"/>
+      <c r="G59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A60" s="104"/>
+      <c r="A60" s="87"/>
       <c r="B60" s="50" t="s">
         <v>8</v>
       </c>
@@ -2286,10 +2313,10 @@
       <c r="D60" s="2"/>
       <c r="E60" s="4"/>
       <c r="F60" s="16"/>
-      <c r="G60" s="87"/>
+      <c r="G60" s="106"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="105">
+      <c r="A61" s="88">
         <v>6</v>
       </c>
       <c r="B61" s="35" t="s">
@@ -2299,39 +2326,39 @@
       <c r="D61" s="36"/>
       <c r="E61" s="37"/>
       <c r="F61" s="37"/>
-      <c r="G61" s="88"/>
+      <c r="G61" s="107"/>
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A62" s="105"/>
-      <c r="B62" s="77" t="s">
+      <c r="A62" s="88"/>
+      <c r="B62" s="78" t="s">
         <v>44</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="4"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="89"/>
+      <c r="G62" s="108"/>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="105"/>
-      <c r="B63" s="77"/>
+      <c r="A63" s="88"/>
+      <c r="B63" s="78"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="4"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="89"/>
+      <c r="G63" s="108"/>
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" s="105"/>
-      <c r="B64" s="77"/>
+      <c r="A64" s="88"/>
+      <c r="B64" s="78"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="4"/>
       <c r="F64" s="16"/>
-      <c r="G64" s="89"/>
+      <c r="G64" s="108"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="105"/>
+      <c r="A65" s="88"/>
       <c r="B65" s="50" t="s">
         <v>46</v>
       </c>
@@ -2339,10 +2366,10 @@
       <c r="D65" s="2"/>
       <c r="E65" s="4"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="89"/>
+      <c r="G65" s="108"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="105"/>
+      <c r="A66" s="88"/>
       <c r="B66" s="50" t="s">
         <v>8</v>
       </c>
@@ -2350,10 +2377,10 @@
       <c r="D66" s="2"/>
       <c r="E66" s="4"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="90"/>
+      <c r="G66" s="109"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="106">
+      <c r="A67" s="89">
         <v>7</v>
       </c>
       <c r="B67" s="38" t="s">
@@ -2363,39 +2390,39 @@
       <c r="D67" s="39"/>
       <c r="E67" s="40"/>
       <c r="F67" s="41"/>
-      <c r="G67" s="81"/>
+      <c r="G67" s="101"/>
     </row>
     <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A68" s="106"/>
-      <c r="B68" s="77" t="s">
+      <c r="A68" s="89"/>
+      <c r="B68" s="78" t="s">
         <v>44</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="4"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="82"/>
+      <c r="G68" s="102"/>
     </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="106"/>
-      <c r="B69" s="77"/>
+      <c r="A69" s="89"/>
+      <c r="B69" s="78"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="4"/>
       <c r="F69" s="16"/>
-      <c r="G69" s="82"/>
+      <c r="G69" s="102"/>
     </row>
     <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A70" s="106"/>
-      <c r="B70" s="77"/>
+      <c r="A70" s="89"/>
+      <c r="B70" s="78"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="4"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="82"/>
+      <c r="G70" s="102"/>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A71" s="106"/>
+      <c r="A71" s="89"/>
       <c r="B71" s="50" t="s">
         <v>46</v>
       </c>
@@ -2403,10 +2430,10 @@
       <c r="D71" s="2"/>
       <c r="E71" s="4"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="82"/>
+      <c r="G71" s="102"/>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="106"/>
+      <c r="A72" s="89"/>
       <c r="B72" s="50" t="s">
         <v>8</v>
       </c>
@@ -2414,10 +2441,10 @@
       <c r="D72" s="2"/>
       <c r="E72" s="4"/>
       <c r="F72" s="16"/>
-      <c r="G72" s="83"/>
+      <c r="G72" s="103"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="107">
+      <c r="A73" s="81">
         <v>8</v>
       </c>
       <c r="B73" s="42" t="s">
@@ -2427,30 +2454,30 @@
       <c r="D73" s="43"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
-      <c r="G73" s="78"/>
+      <c r="G73" s="98"/>
     </row>
     <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A74" s="107"/>
-      <c r="B74" s="77" t="s">
+      <c r="A74" s="81"/>
+      <c r="B74" s="78" t="s">
         <v>44</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="4"/>
       <c r="F74" s="16"/>
-      <c r="G74" s="79"/>
+      <c r="G74" s="99"/>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A75" s="107"/>
-      <c r="B75" s="77"/>
+      <c r="A75" s="81"/>
+      <c r="B75" s="78"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="4"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="79"/>
+      <c r="G75" s="99"/>
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A76" s="107"/>
+      <c r="A76" s="81"/>
       <c r="B76" s="50" t="s">
         <v>7</v>
       </c>
@@ -2458,10 +2485,10 @@
       <c r="D76" s="2"/>
       <c r="E76" s="4"/>
       <c r="F76" s="16"/>
-      <c r="G76" s="79"/>
+      <c r="G76" s="99"/>
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A77" s="107"/>
+      <c r="A77" s="81"/>
       <c r="B77" s="50" t="s">
         <v>46</v>
       </c>
@@ -2469,10 +2496,10 @@
       <c r="D77" s="2"/>
       <c r="E77" s="4"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="79"/>
+      <c r="G77" s="99"/>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A78" s="107"/>
+      <c r="A78" s="81"/>
       <c r="B78" s="50" t="s">
         <v>8</v>
       </c>
@@ -2480,10 +2507,10 @@
       <c r="D78" s="2"/>
       <c r="E78" s="4"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="80"/>
+      <c r="G78" s="100"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="67">
+      <c r="A79" s="84">
         <v>9</v>
       </c>
       <c r="B79" s="12" t="s">
@@ -2493,39 +2520,39 @@
       <c r="D79" s="13"/>
       <c r="E79" s="14"/>
       <c r="F79" s="15"/>
-      <c r="G79" s="108"/>
+      <c r="G79" s="69"/>
     </row>
     <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A80" s="67"/>
-      <c r="B80" s="77" t="s">
+      <c r="A80" s="84"/>
+      <c r="B80" s="78" t="s">
         <v>44</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="4"/>
       <c r="F80" s="16"/>
-      <c r="G80" s="109"/>
+      <c r="G80" s="70"/>
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A81" s="67"/>
-      <c r="B81" s="77"/>
+      <c r="A81" s="84"/>
+      <c r="B81" s="78"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="4"/>
       <c r="F81" s="16"/>
-      <c r="G81" s="109"/>
+      <c r="G81" s="70"/>
     </row>
     <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A82" s="67"/>
-      <c r="B82" s="77"/>
+      <c r="A82" s="84"/>
+      <c r="B82" s="78"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="4"/>
       <c r="F82" s="16"/>
-      <c r="G82" s="109"/>
+      <c r="G82" s="70"/>
     </row>
     <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A83" s="67"/>
+      <c r="A83" s="84"/>
       <c r="B83" s="50" t="s">
         <v>7</v>
       </c>
@@ -2533,10 +2560,10 @@
       <c r="D83" s="2"/>
       <c r="E83" s="4"/>
       <c r="F83" s="16"/>
-      <c r="G83" s="109"/>
+      <c r="G83" s="70"/>
     </row>
     <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A84" s="67"/>
+      <c r="A84" s="84"/>
       <c r="B84" s="50" t="s">
         <v>46</v>
       </c>
@@ -2544,10 +2571,10 @@
       <c r="D84" s="2"/>
       <c r="E84" s="4"/>
       <c r="F84" s="16"/>
-      <c r="G84" s="109"/>
+      <c r="G84" s="70"/>
     </row>
     <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A85" s="67"/>
+      <c r="A85" s="84"/>
       <c r="B85" s="50" t="s">
         <v>8</v>
       </c>
@@ -2555,10 +2582,10 @@
       <c r="D85" s="2"/>
       <c r="E85" s="4"/>
       <c r="F85" s="16"/>
-      <c r="G85" s="110"/>
+      <c r="G85" s="71"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="84">
+      <c r="A86" s="83">
         <v>10</v>
       </c>
       <c r="B86" s="46" t="s">
@@ -2568,30 +2595,30 @@
       <c r="D86" s="47"/>
       <c r="E86" s="19"/>
       <c r="F86" s="20"/>
-      <c r="G86" s="111"/>
+      <c r="G86" s="72"/>
     </row>
     <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A87" s="84"/>
-      <c r="B87" s="96" t="s">
+      <c r="A87" s="83"/>
+      <c r="B87" s="79" t="s">
         <v>44</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="4"/>
       <c r="F87" s="16"/>
-      <c r="G87" s="112"/>
+      <c r="G87" s="73"/>
     </row>
     <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A88" s="84"/>
-      <c r="B88" s="98"/>
+      <c r="A88" s="83"/>
+      <c r="B88" s="80"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="4"/>
       <c r="F88" s="16"/>
-      <c r="G88" s="112"/>
+      <c r="G88" s="73"/>
     </row>
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A89" s="84"/>
+      <c r="A89" s="83"/>
       <c r="B89" s="50" t="s">
         <v>7</v>
       </c>
@@ -2599,10 +2626,10 @@
       <c r="D89" s="2"/>
       <c r="E89" s="4"/>
       <c r="F89" s="16"/>
-      <c r="G89" s="112"/>
+      <c r="G89" s="73"/>
     </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A90" s="84"/>
+      <c r="A90" s="83"/>
       <c r="B90" s="50" t="s">
         <v>46</v>
       </c>
@@ -2610,10 +2637,10 @@
       <c r="D90" s="2"/>
       <c r="E90" s="4"/>
       <c r="F90" s="16"/>
-      <c r="G90" s="112"/>
+      <c r="G90" s="73"/>
     </row>
     <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A91" s="84"/>
+      <c r="A91" s="83"/>
       <c r="B91" s="50" t="s">
         <v>8</v>
       </c>
@@ -2621,10 +2648,10 @@
       <c r="D91" s="2"/>
       <c r="E91" s="4"/>
       <c r="F91" s="16"/>
-      <c r="G91" s="113"/>
+      <c r="G91" s="74"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="68">
+      <c r="A92" s="75">
         <v>11</v>
       </c>
       <c r="B92" s="21" t="s">
@@ -2636,13 +2663,13 @@
       <c r="D92" s="22"/>
       <c r="E92" s="23"/>
       <c r="F92" s="24"/>
-      <c r="G92" s="68" t="s">
+      <c r="G92" s="75" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A93" s="69"/>
-      <c r="B93" s="97" t="s">
+      <c r="A93" s="76"/>
+      <c r="B93" s="82" t="s">
         <v>44</v>
       </c>
       <c r="C93" s="52" t="s">
@@ -2655,11 +2682,11 @@
       <c r="F93" s="16">
         <v>43919</v>
       </c>
-      <c r="G93" s="69"/>
+      <c r="G93" s="76"/>
     </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A94" s="69"/>
-      <c r="B94" s="97"/>
+      <c r="A94" s="76"/>
+      <c r="B94" s="82"/>
       <c r="C94" s="52" t="s">
         <v>14</v>
       </c>
@@ -2670,11 +2697,11 @@
       <c r="F94" s="16">
         <v>43916</v>
       </c>
-      <c r="G94" s="69"/>
+      <c r="G94" s="76"/>
     </row>
     <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A95" s="69"/>
-      <c r="B95" s="97"/>
+      <c r="A95" s="76"/>
+      <c r="B95" s="82"/>
       <c r="C95" s="52" t="s">
         <v>15</v>
       </c>
@@ -2685,11 +2712,11 @@
       <c r="F95" s="16">
         <v>43915</v>
       </c>
-      <c r="G95" s="69"/>
+      <c r="G95" s="76"/>
     </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A96" s="69"/>
-      <c r="B96" s="97"/>
+      <c r="A96" s="76"/>
+      <c r="B96" s="82"/>
       <c r="C96" s="52" t="s">
         <v>16</v>
       </c>
@@ -2700,11 +2727,11 @@
       <c r="F96" s="16">
         <v>43920</v>
       </c>
-      <c r="G96" s="69"/>
+      <c r="G96" s="76"/>
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A97" s="69"/>
-      <c r="B97" s="97"/>
+      <c r="A97" s="76"/>
+      <c r="B97" s="82"/>
       <c r="C97" s="52" t="s">
         <v>17</v>
       </c>
@@ -2715,11 +2742,11 @@
       <c r="F97" s="16">
         <v>43931</v>
       </c>
-      <c r="G97" s="69"/>
+      <c r="G97" s="76"/>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A98" s="69"/>
-      <c r="B98" s="97"/>
+      <c r="A98" s="76"/>
+      <c r="B98" s="82"/>
       <c r="C98" s="52" t="s">
         <v>18</v>
       </c>
@@ -2730,11 +2757,11 @@
       <c r="F98" s="16">
         <v>43931</v>
       </c>
-      <c r="G98" s="69"/>
+      <c r="G98" s="76"/>
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A99" s="69"/>
-      <c r="B99" s="97"/>
+      <c r="A99" s="76"/>
+      <c r="B99" s="82"/>
       <c r="C99" s="52" t="s">
         <v>19</v>
       </c>
@@ -2745,10 +2772,10 @@
       <c r="F99" s="16">
         <v>43931</v>
       </c>
-      <c r="G99" s="69"/>
+      <c r="G99" s="76"/>
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A100" s="69"/>
+      <c r="A100" s="76"/>
       <c r="B100" s="53" t="s">
         <v>7</v>
       </c>
@@ -2758,10 +2785,10 @@
         <v>1</v>
       </c>
       <c r="F100" s="16"/>
-      <c r="G100" s="69"/>
+      <c r="G100" s="76"/>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A101" s="69"/>
+      <c r="A101" s="76"/>
       <c r="B101" s="53" t="s">
         <v>46</v>
       </c>
@@ -2773,10 +2800,10 @@
       <c r="F101" s="16">
         <v>43928</v>
       </c>
-      <c r="G101" s="69"/>
+      <c r="G101" s="76"/>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A102" s="70"/>
+      <c r="A102" s="77"/>
       <c r="B102" s="53" t="s">
         <v>8</v>
       </c>
@@ -2788,37 +2815,16 @@
       <c r="F102" s="16">
         <v>43928</v>
       </c>
-      <c r="G102" s="70"/>
+      <c r="G102" s="77"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F2" xr:uid="{60BF8AA0-547A-4AC4-BE58-D9F0611612D0}"/>
   <mergeCells count="43">
-    <mergeCell ref="G79:G85"/>
-    <mergeCell ref="G86:G91"/>
-    <mergeCell ref="G92:G102"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="A73:A78"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A92:A102"/>
-    <mergeCell ref="B93:B99"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="A39:A46"/>
-    <mergeCell ref="A47:A54"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="A67:A72"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="A19:A29"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B9:B16"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B20:B27"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="G3:G7"/>
+    <mergeCell ref="G8:G18"/>
+    <mergeCell ref="G30:G38"/>
+    <mergeCell ref="G39:G46"/>
+    <mergeCell ref="G47:G54"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="G73:G78"/>
     <mergeCell ref="G67:G72"/>
@@ -2831,11 +2837,32 @@
     <mergeCell ref="B74:B75"/>
     <mergeCell ref="D20:D29"/>
     <mergeCell ref="D31:D38"/>
-    <mergeCell ref="G3:G7"/>
-    <mergeCell ref="G8:G18"/>
-    <mergeCell ref="G30:G38"/>
-    <mergeCell ref="G39:G46"/>
-    <mergeCell ref="G47:G54"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="A19:A29"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B9:B16"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="A47:A54"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="A67:A72"/>
+    <mergeCell ref="A73:A78"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A92:A102"/>
+    <mergeCell ref="B93:B99"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="G79:G85"/>
+    <mergeCell ref="G86:G91"/>
+    <mergeCell ref="G92:G102"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B87:B88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>